<commit_message>
new changes for oauth, bot detection, file upload
</commit_message>
<xml_diff>
--- a/testData/amazonSteps - Copy.xlsx
+++ b/testData/amazonSteps - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_GenAI/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_Playwright_GenAI/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{D98CA4CA-DDC4-4ED3-856D-28D5CDCC6857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD053F69-FFB1-445D-93E3-40F9D45761E2}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29AD15B9-4B88-4901-A10A-105C74E80185}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>action</t>
   </si>
@@ -48,18 +48,27 @@
     <t>https://www.amazon.com/</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>press</t>
+  </si>
+  <si>
+    <t>Enter key</t>
+  </si>
+  <si>
     <t>click</t>
   </si>
   <si>
     <t>Hello, Sign in</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>email input field</t>
   </si>
   <si>
+    <t>weavernormar@gmail.com</t>
+  </si>
+  <si>
     <t>Continue button on page</t>
   </si>
   <si>
@@ -72,52 +81,52 @@
     <t>signin button on page</t>
   </si>
   <si>
-    <t>Search input field</t>
-  </si>
-  <si>
-    <t>press</t>
-  </si>
-  <si>
-    <t>scroll</t>
+    <t>https://www.amazon.com/gp/cart/view.html?ref_=nav_cart</t>
+  </si>
+  <si>
+    <t>assert</t>
+  </si>
+  <si>
+    <t>h2#deliver-to-customer-text</t>
+  </si>
+  <si>
+    <t>Delivering to Normar Weaver</t>
+  </si>
+  <si>
+    <t>waitfortext</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>scrollto</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>checkvisible</t>
+  </si>
+  <si>
+    <t>Search Amazon</t>
+  </si>
+  <si>
+    <t>pressto</t>
   </si>
   <si>
     <t>chair</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/cart/view.html?ref_=nav_cart</t>
-  </si>
-  <si>
-    <t>assert</t>
-  </si>
-  <si>
-    <t>h2#deliver-to-customer-text</t>
-  </si>
-  <si>
-    <t>Delivering to Normar Weaver</t>
-  </si>
-  <si>
-    <t>nclick</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>Add to Cart</t>
-  </si>
-  <si>
-    <t>weavernormar@gmail.com</t>
-  </si>
-  <si>
-    <t>Proceed to checkout</t>
-  </si>
-  <si>
-    <t>waitfortext</t>
-  </si>
-  <si>
-    <t>Payment method</t>
-  </si>
-  <si>
-    <t>Enter key</t>
+    <t>Add to cart</t>
+  </si>
+  <si>
+    <t>input[name="proceedToRetailCheckout"]</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>clickto</t>
   </si>
 </sst>
 </file>
@@ -451,9 +460,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -495,60 +506,48 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2000</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1">
-        <v>3000</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1">
-        <v>1000</v>
-      </c>
       <c r="E6" s="1">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -559,41 +558,41 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1">
         <v>1000</v>
       </c>
       <c r="E8" s="1">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D10" s="1">
         <v>1000</v>
@@ -604,10 +603,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="E11" s="1">
         <v>2000</v>
@@ -615,110 +617,86 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E12" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1000</v>
       </c>
       <c r="E13" s="1">
-        <v>3000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1000</v>
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="E14" s="1">
-        <v>2000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1000</v>
+        <v>32</v>
       </c>
       <c r="E15" s="1">
-        <v>2000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E16" s="1">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E18" s="1">
-        <v>2000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{4D1D879C-C7A8-4E1E-94C1-03083C83B40F}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{3F758E2D-457F-4F4D-BB11-70AD9C1813E6}"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{BA0E224C-C858-47AF-8859-A659DB8B5C6D}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{AB3D6231-B488-4B94-BF6C-F9D8D7D5C450}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{3639D1C9-3665-45CB-ACD0-65478BA24DD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new changes for multiple retailers and allure reporting
</commit_message>
<xml_diff>
--- a/testData/amazonSteps - Copy.xlsx
+++ b/testData/amazonSteps - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_Playwright_GenAI/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29AD15B9-4B88-4901-A10A-105C74E80185}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="6_{57788A50-2754-4C97-9C7B-071C8F708F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC994881-2A7E-461F-948F-905A7F08528E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>action</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>clickto</t>
+  </si>
+  <si>
+    <t>the first Use this address button</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,12 +684,20 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>